<commit_message>
removed for loop in image detect
</commit_message>
<xml_diff>
--- a/static/debugger_log.xlsx
+++ b/static/debugger_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="10">
   <si>
     <t>Object Detection</t>
   </si>
@@ -35,6 +35,15 @@
   </si>
   <si>
     <t>23/04/2022 12:57:33 AM</t>
+  </si>
+  <si>
+    <t>Exception: Update image directory</t>
+  </si>
+  <si>
+    <t>[Errno 13] Permission denied: 'c:\\Users\\user10\\Desktop\\Hobby\\Programming\\EEEY3 Project\\Web App\\Elephant_Web_App_v2\\static/image uploads/end device 2/2021-09-15 16-18-18-x-whale - Copy.jpg'</t>
+  </si>
+  <si>
+    <t>07/05/2022 03:36:31 AM</t>
   </si>
 </sst>
 </file>
@@ -366,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -680,6 +689,34 @@
         <v>6</v>
       </c>
     </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>